<commit_message>
Added more options for creation of design matrix, and senstype ref.
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/config/design_input_example1.xlsx
+++ b/tests/data/sensitivities/config/design_input_example1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -120,7 +120,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>For case sensitivitiesprovide names for case1 and case2 and values. Values can be string</t>
+          <t>For scenario sensitivities provide names for case1 and case2 and values. Values can be string or numbers</t>
         </r>
       </text>
     </comment>
@@ -134,11 +134,14 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Distname and dist_param1, .. only for monte carlo sensitivities. Order of distribution parameters is predefined: 
-normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
-lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
-uniform(from,to)loguniform(from, to)triangular(low, mode, high)
-discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n))</t>
+          <t>Distname and dist_param1, .. only for sensitivities of type “dist”. 
+The order of distribution parameters is predefined: 
+normal(mean, std dev,min, max)     – where min/max is optional and will give truncated gaussian
+lognormal(mean, stddev) 
+uniform(from,to)
+loguniform(from, to)
+triangular(low, mode, high)
+discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n)). Discrete uniform if no weights are given</t>
         </r>
       </text>
     </comment>
@@ -172,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>designtype</t>
   </si>
@@ -207,13 +210,13 @@
     <t>param_name</t>
   </si>
   <si>
-    <t>senscase1</t>
+    <t>casename1</t>
   </si>
   <si>
     <t>value1</t>
   </si>
   <si>
-    <t>senscase2</t>
+    <t>casename2</t>
   </si>
   <si>
     <t>value2</t>
@@ -243,88 +246,91 @@
     <t>extern_file</t>
   </si>
   <si>
+    <t>rms_seed</t>
+  </si>
+  <si>
     <t>seed</t>
   </si>
   <si>
+    <t>faults</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>FAULT_POSITION</t>
+  </si>
+  <si>
+    <t>east</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>velmodel</t>
+  </si>
+  <si>
+    <t>DC_MODEL</t>
+  </si>
+  <si>
+    <t>alternative</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>OWC1</t>
+  </si>
+  <si>
+    <t>shallow</t>
+  </si>
+  <si>
+    <t>deep</t>
+  </si>
+  <si>
+    <t>OWC2</t>
+  </si>
+  <si>
+    <t>OWC3</t>
+  </si>
+  <si>
+    <t>multz</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>MULTZ_ILE</t>
+  </si>
+  <si>
+    <t>logunif</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
     <t>RMS_SEED</t>
   </si>
   <si>
-    <t>faults</t>
-  </si>
-  <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>fault_position</t>
-  </si>
-  <si>
-    <t>east</t>
-  </si>
-  <si>
-    <t>west</t>
-  </si>
-  <si>
-    <t>velmodel</t>
-  </si>
-  <si>
-    <t>dc_model</t>
-  </si>
-  <si>
-    <t>alternative</t>
-  </si>
-  <si>
-    <t>contacts</t>
-  </si>
-  <si>
-    <t>owc1</t>
-  </si>
-  <si>
-    <t>shallow</t>
-  </si>
-  <si>
-    <t>deep</t>
-  </si>
-  <si>
-    <t>owc2</t>
-  </si>
-  <si>
-    <t>owc3</t>
-  </si>
-  <si>
-    <t>multz</t>
-  </si>
-  <si>
-    <t>dist</t>
-  </si>
-  <si>
-    <t>multz_ile</t>
-  </si>
-  <si>
-    <t>logunif</t>
-  </si>
-  <si>
-    <t>0.0001</t>
-  </si>
-  <si>
-    <t>default_value</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
-    <t>param1</t>
-  </si>
-  <si>
-    <t>param2</t>
+    <t>PARAM1</t>
+  </si>
+  <si>
+    <t>PARAM2</t>
   </si>
   <si>
     <t>0.1</t>
   </si>
   <si>
-    <t>param3</t>
-  </si>
-  <si>
-    <t>param4</t>
+    <t>PARAM3</t>
+  </si>
+  <si>
+    <t>PARAM4</t>
   </si>
 </sst>
 </file>
@@ -962,7 +968,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1014,7 +1020,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1070,7 +1076,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1412,8 +1418,8 @@
   </sheetPr>
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q35" activeCellId="0" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1421,7 +1427,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8520408163265"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1887755102041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.8622448979592"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.8469387755102"/>
@@ -1494,11 +1500,9 @@
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="20" t="s">
         <v>24</v>
       </c>
+      <c r="D2" s="20"/>
       <c r="E2" s="21"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
@@ -1703,8 +1707,8 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1724,7 +1728,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="109" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1000</v>
@@ -1743,7 +1747,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1784,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="110" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>0</v>
@@ -1788,15 +1792,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="110" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="110" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0</v>
@@ -1804,7 +1808,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="110" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
revert casename to senscase
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/config/design_input_example1.xlsx
+++ b/tests/data/sensitivities/config/design_input_example1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -210,13 +210,13 @@
     <t>param_name</t>
   </si>
   <si>
-    <t>casename1</t>
+    <t>senscase1</t>
   </si>
   <si>
     <t>value1</t>
   </si>
   <si>
-    <t>casename2</t>
+    <t>senscase2</t>
   </si>
   <si>
     <t>value2</t>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q35" activeCellId="0" sqref="Q35"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Reorganisation of code to allow for several correlation matrices per sensitivity. Needed for full montecarlo studies to avoid very large correlation matrices. Can now use several smaller instead when only groups of parameters are correlated. Change in designsheet specification: Have to specify corr_sheet for every correlated parameter.
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/config/design_input_example1.xlsx
+++ b/tests/data/sensitivities/config/design_input_example1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,16 +23,60 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="B2" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="B3" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="B4" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -45,13 +89,46 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="E1" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="I1" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -64,7 +141,18 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t> </t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -1244,7 +1332,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1296,6 +1384,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1306,8 +1395,8 @@
   </sheetPr>
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="7:7 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1584,6 +1673,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1594,8 +1684,8 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1709,5 +1799,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>